<commit_message>
Latest code and TechStack updated
</commit_message>
<xml_diff>
--- a/TechStack.xlsx
+++ b/TechStack.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9529DD23-5A1E-4F2B-BB22-025ED1DDA427}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42324789-FA50-49D7-9E0F-36D7655E9A96}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="979" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="979" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="About Author" sheetId="19" r:id="rId1"/>
-    <sheet name="SDLC" sheetId="17" r:id="rId2"/>
+    <sheet name="SDLC" sheetId="17" r:id="rId1"/>
+    <sheet name="Solid Principles" sheetId="19" r:id="rId2"/>
     <sheet name="Core Java" sheetId="1" r:id="rId3"/>
     <sheet name="Design Patterns" sheetId="18" r:id="rId4"/>
     <sheet name="Spring" sheetId="2" r:id="rId5"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="745" uniqueCount="704">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="792" uniqueCount="743">
   <si>
     <t>Topic</t>
   </si>
@@ -3691,9 +3691,6 @@
     </r>
   </si>
   <si>
-    <t>Requirements</t>
-  </si>
-  <si>
     <t>Analysis</t>
   </si>
   <si>
@@ -3701,9 +3698,6 @@
   </si>
   <si>
     <t>Implementation</t>
-  </si>
-  <si>
-    <t>Test</t>
   </si>
   <si>
     <t xml:space="preserve">What are the different testing phases involved in your project?
@@ -5447,18 +5441,6 @@
     <t>Describe Some of the Functional Interfaces in the Standard Library.</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>Rajendra</t>
-  </si>
-  <si>
-    <t>Email</t>
-  </si>
-  <si>
-    <t>Rajendra.lella@live.com</t>
-  </si>
-  <si>
     <t xml:space="preserve">one to one (Every Citizen has a Unique Aadhaar)/(Every Tax payer has a Unique PAN card)
 one to many (Author to Books)
 many to one (Books to Author)
@@ -5929,84 +5911,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">ClassLoader always follows the Delegation Hierarchy Principle.
-Whenever JVM comes across a class, it checks whether that class is already loaded or not.
-If the Class is already loaded in the method area then the JVM proceeds with execution.
-If the class is not present in the method area then the JVM asks the Java ClassLoader Sub-System to load that particular class, then ClassLoader sub-system hands over the control to Application ClassLoader.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Application ClassLoader</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> then delegates the request to Extension ClassLoader and the Extension ClassLoader in turn delegates the request to Bootstrap ClassLoader.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Bootstrap ClassLoader</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> will search in the Bootstrap classpath(JDK/JRE/LIB). If the class is available then it is loaded, if not the request is delegated to Extension ClassLoader.
-</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Extension ClassLoader</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> searches for the class in the Extension Classpath(JDK/JRE/LIB/EXT). If the class is available then it is loaded, if not the request is delegated to the Application ClassLoader.
-Application ClassLoader searches for the class in the Application Classpath. If the class is available then it is loaded, if not then a ClassNotFoundException exception is generated</t>
-    </r>
-  </si>
-  <si>
     <t xml:space="preserve">Factory Desgin Pattern:
 </t>
   </si>
@@ -6122,12 +6026,306 @@
   <si>
     <t>Singleton Design Pattern:</t>
   </si>
+  <si>
+    <t>Requirements Planning</t>
+  </si>
+  <si>
+    <t>Test &amp; Integration</t>
+  </si>
+  <si>
+    <t>Why pointers are not used in java?</t>
+  </si>
+  <si>
+    <t>Java allocates memory implicitly and giving direct access to memory to the users can lead to memory management issues, hence pointers are discouraged in java.</t>
+  </si>
+  <si>
+    <t>What's the advantage of using getters and setters that only get and set instead of simply using public fields for those variables?</t>
+  </si>
+  <si>
+    <t>One advantage of accessors and mutators is that you can perform validation. For example, if foo was public, I could easily set it to null and then someone else could try to call a method on the object.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Question </t>
+  </si>
+  <si>
+    <t>What is SOLID Principle?</t>
+  </si>
+  <si>
+    <t>SOLID Principles is a coding standard that helps us to have a clear concept for developing software properly to avoid a bad design. It was promoted by Robert C Martin and is used across the object-oriented design spectrum. When applied properly it makes our code more extendable, logical, and easier to read.</t>
+  </si>
+  <si>
+    <t>Single Responsibility Principle</t>
+  </si>
+  <si>
+    <t>A class should have one and only one responsibility</t>
+  </si>
+  <si>
+    <t>Actual Implemenation</t>
+  </si>
+  <si>
+    <t>public class PrintStudent{
+ public void printDetails(){
+ }
+}</t>
+  </si>
+  <si>
+    <t>public class CalculateStudentPercentage{
+ public void calculatePercentageDetails(){(){
+ }
+}</t>
+  </si>
+  <si>
+    <t>public class AddStudent{
+ public void addStudent(){
+ }
+}</t>
+  </si>
+  <si>
+    <t>Open Closed Principle</t>
+  </si>
+  <si>
+    <t>A class should be open for extension and closed for modification</t>
+  </si>
+  <si>
+    <t>public interface Vehicle{
+  public String getVechicleNo();
+}</t>
+  </si>
+  <si>
+    <t>public class Car extends Vehicle{
+  public String getVehicleNo(){
+  }
+}</t>
+  </si>
+  <si>
+    <t>public class Bike extends Vehicle{
+  public String getVehicleNo(){
+  }
+}</t>
+  </si>
+  <si>
+    <t>public class Truck extends Vehicle{
+  public String getVehicleNo(){
+  }
+}</t>
+  </si>
+  <si>
+    <t>Liskov's Substitution Principle</t>
+  </si>
+  <si>
+    <t>So considering above example, we can code like given below
+Vehicle car = new Car();
+Vehicle bike = new Bike();
+Vehicle truck = new Truck();</t>
+  </si>
+  <si>
+    <t>Interface segregation Principle</t>
+  </si>
+  <si>
+    <t>This principle tells us that large interfaces should be split into smaller onces, Because the implementation classes consider only what is required. We should not force the clients to provide dummy implementation for the classes which are not required to implement.</t>
+  </si>
+  <si>
+    <t>public interface Conversion{
+ public void intToDouble();
+ public void intToChar();
+ public void intToString();
+}</t>
+  </si>
+  <si>
+    <t>So in the above example if any one who is required to implement intToDouble() only, he has to implement the other two methods also for sure</t>
+  </si>
+  <si>
+    <t>To over come the issue, below is the implemenation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">public class Student{
+   public void printDetails(){
+   }
+  public void calculatePercentageDetails(){
+   }
+  public void addStudent(){
+   }
+}
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Below code is violation of Single Responsibility </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">public class Vehicle{
+   public String getVehicleDetails(Vechicle vehicle){
+     if(vehicle instanceOf Car){
+       return vehicle.getVehicleNo();
+     } else if(vehicle instanceOf Bike){
+       return vehicle.getVechicleNo();
+     } else if (vehicle instanceOf Truck){
+       return vehicle.getVehicleNo();
+     }
+   }
+}
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Note: If we want to add a new vehicle, it will against to open closed principle</t>
+    </r>
+  </si>
+  <si>
+    <t>Ex: Below one is the bad implementation</t>
+  </si>
+  <si>
+    <t>public interface IntToDouble{
+ public void intToDouble();
+}
+public interface IntToChar{
+  public void intToChar();
+}
+public interface IntToString{
+  public  void intToString();
+}</t>
+  </si>
+  <si>
+    <t>Now the fat or bulk implementation is splited to multiple interfaces, which allows the developers to concentrate only on the required ones.</t>
+  </si>
+  <si>
+    <t>Dependency Inversion Principle</t>
+  </si>
+  <si>
+    <t>This applies to inheritance in such a way that the derived classes must be completely substitutable for their base class and should not deviate the basic purpose of the class.
+It concentrates more on IS-A relationship.</t>
+  </si>
+  <si>
+    <t>This principle tells us that high level modules should not depend on low level modules, This also informs us  that we should not make use of the new keyword. Using the new keyword makes he code more tightly coupled.</t>
+  </si>
+  <si>
+    <t>public class WindowsMachine{
+ public final Keyboard keyboard;
+ public final Mouse mouse;
+ public WindowsMachine(){
+    keyboard = new Keyboard();
+    mouse = new Mouse(); 
+  }
+}</t>
+  </si>
+  <si>
+    <t>Violation</t>
+  </si>
+  <si>
+    <t>public class WindowsMachine{
+ public final Keyboard keyboard;
+ public final Mouse mouse;
+ public WindowsMachine(Keyboard kb,Mouse ms){
+   this.keyboard = kb;
+   this.mouse = ms;
+  }
+}</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>L</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">ClassLoader always follows the Delegation Hierarchy Principle.
+Whenever JVM comes across a class, it checks whether that class is already loaded or not.
+If the Class is already loaded in the method area then the JVM proceeds with execution.
+If the class is not present in the method area then the JVM asks the Java ClassLoader Sub-System to load that particular class, then ClassLoader sub-system hands over the control to Application ClassLoader.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Application ClassLoader</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> then delegates the request to Extension ClassLoader and the Extension ClassLoader in turn delegates the request to Bootstrap ClassLoader.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Extension ClassLoader</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> searches for the class in the Extension Classpath(JDK/JRE/LIB/EXT). If the class is available then it is loaded, if not the request is delegated to the Application ClassLoader.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bootstrap ClassLoader</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> will search in the Bootstrap classpath(JDK/JRE/LIB). If the class is available then it is loaded, if not the request is delegated to Extension ClassLoader.
+Application ClassLoader searches for the class in the Application Classpath. If the class is available then it is loaded, if not then a ClassNotFoundException exception is generated</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6260,8 +6458,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6286,8 +6498,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="8">
     <border>
       <left/>
       <right/>
@@ -6373,12 +6595,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -6477,6 +6710,24 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -6492,32 +6743,43 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="0" xfId="2" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="6" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -6535,6 +6797,72 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>22672</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>365759</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>121919</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>91438</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1" descr="Software Development Life Cycle (SDLC) phases | by Jilvan Pinheiro | Medium">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{328359CC-4C8C-4E7B-88F3-153F3E77AE45}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8549452" y="365759"/>
+          <a:ext cx="4976047" cy="2796539"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -6639,7 +6967,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -6694,7 +7022,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
@@ -7022,39 +7350,68 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E9AD4CB-F1AE-4B35-B8C1-FA2098014754}">
-  <dimension ref="C7:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADC389A-9F0E-41B8-8C1E-C0071BC3B5C1}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="31"/>
+    <col min="2" max="2" width="115.44140625" style="31" customWidth="1"/>
+    <col min="3" max="16384" width="8.88671875" style="31"/>
   </cols>
   <sheetData>
-    <row r="7" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C7" s="37" t="s">
-        <v>664</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="8" spans="3:4" x14ac:dyDescent="0.3">
-      <c r="C8" s="37" t="s">
-        <v>666</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>667</v>
+    <row r="1" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="31" t="s">
+        <v>553</v>
+      </c>
+      <c r="B1" s="32" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="198.6" x14ac:dyDescent="0.3">
+      <c r="B2" s="33" t="s">
+        <v>554</v>
+      </c>
+      <c r="D2"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B3" s="31" t="s">
+        <v>697</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B4" s="31" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B5" s="31" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B6" s="31" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B7" s="31" t="s">
+        <v>698</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B8" s="32" t="s">
+        <v>558</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D8" r:id="rId1" xr:uid="{3BBFB07B-82CD-4E96-979D-295F88C7C989}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -7150,12 +7507,12 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>671</v>
+        <v>665</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>672</v>
+        <v>666</v>
       </c>
     </row>
   </sheetData>
@@ -7198,10 +7555,10 @@
     </row>
     <row r="3" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B3" s="10" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
       <c r="C3" s="11" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="72" x14ac:dyDescent="0.3">
@@ -7209,23 +7566,23 @@
         <v>16</v>
       </c>
       <c r="C4" s="11" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="5" spans="1:4" s="29" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B5" s="11" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
       <c r="C5" s="11" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="115.2" x14ac:dyDescent="0.3">
       <c r="B6" s="11" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
       <c r="C6" s="11" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="144" x14ac:dyDescent="0.3">
@@ -7233,7 +7590,7 @@
         <v>17</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
       <c r="D7"/>
     </row>
@@ -7345,7 +7702,7 @@
         <v>0</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -7362,7 +7719,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
       <c r="C3" s="1"/>
     </row>
@@ -7532,7 +7889,7 @@
         <v>19</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
       <c r="C25" s="1"/>
     </row>
@@ -8533,10 +8890,10 @@
         <v>22</v>
       </c>
       <c r="B23" s="6" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
@@ -8612,64 +8969,283 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADC389A-9F0E-41B8-8C1E-C0071BC3B5C1}">
-  <dimension ref="A1:B8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E9AD4CB-F1AE-4B35-B8C1-FA2098014754}">
+  <dimension ref="A1:D27"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B25" sqref="B25:B27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="15.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="31"/>
-    <col min="2" max="2" width="115.44140625" style="31" customWidth="1"/>
-    <col min="3" max="16384" width="8.88671875" style="31"/>
+    <col min="1" max="1" width="4.88671875" style="9" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.109375" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="77" style="9" customWidth="1"/>
+    <col min="4" max="4" width="44" style="9" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="15.77734375" style="9"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A1" s="31" t="s">
-        <v>553</v>
-      </c>
-      <c r="B1" s="32" t="s">
-        <v>569</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="198.6" x14ac:dyDescent="0.3">
-      <c r="B2" s="33" t="s">
-        <v>554</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B3" s="31" t="s">
-        <v>555</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B4" s="31" t="s">
-        <v>556</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B5" s="31" t="s">
-        <v>557</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B6" s="31" t="s">
-        <v>558</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="B7" s="31" t="s">
-        <v>559</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="B8" s="32" t="s">
-        <v>560</v>
+    <row r="1" spans="1:4" s="18" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="17" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="57"/>
+      <c r="B2" s="58" t="s">
+        <v>704</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="53" t="s">
+        <v>737</v>
+      </c>
+      <c r="B3" s="53" t="s">
+        <v>706</v>
+      </c>
+      <c r="C3" s="9" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="53"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="54" t="s">
+        <v>726</v>
+      </c>
+      <c r="D4" s="55" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="53"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="52" t="s">
+        <v>725</v>
+      </c>
+      <c r="D5" s="52" t="s">
+        <v>709</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="53"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="51"/>
+      <c r="D6" s="51"/>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="53"/>
+      <c r="B7" s="53"/>
+      <c r="C7" s="51"/>
+      <c r="D7" s="51"/>
+    </row>
+    <row r="8" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="53"/>
+      <c r="B8" s="53"/>
+      <c r="C8" s="51"/>
+      <c r="D8" s="13" t="s">
+        <v>710</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="53"/>
+      <c r="B9" s="53"/>
+      <c r="C9" s="51"/>
+      <c r="D9" s="13" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="53" t="s">
+        <v>738</v>
+      </c>
+      <c r="B10" s="53" t="s">
+        <v>712</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>713</v>
+      </c>
+      <c r="D10" s="55" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="53"/>
+      <c r="B11" s="53"/>
+      <c r="C11" s="52" t="s">
+        <v>727</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="53"/>
+      <c r="B12" s="53"/>
+      <c r="C12" s="51"/>
+      <c r="D12" s="13" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="53"/>
+      <c r="B13" s="53"/>
+      <c r="C13" s="51"/>
+      <c r="D13" s="13" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="53"/>
+      <c r="B14" s="53"/>
+      <c r="C14" s="51"/>
+      <c r="D14" s="13" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="53" t="s">
+        <v>739</v>
+      </c>
+      <c r="B15" s="53" t="s">
+        <v>718</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>732</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="53"/>
+      <c r="B16" s="53"/>
+      <c r="C16" s="13" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="53"/>
+      <c r="B17" s="53"/>
+      <c r="C17" s="13" t="s">
+        <v>715</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="53"/>
+      <c r="B18" s="53"/>
+      <c r="C18" s="13" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="53"/>
+      <c r="B19" s="53"/>
+      <c r="C19" s="13" t="s">
+        <v>717</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="53"/>
+      <c r="B20" s="53"/>
+      <c r="C20" s="13" t="s">
+        <v>719</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="59" t="s">
+        <v>740</v>
+      </c>
+      <c r="B21" s="53" t="s">
+        <v>720</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="59"/>
+      <c r="B22" s="53"/>
+      <c r="C22" s="54" t="s">
+        <v>728</v>
+      </c>
+      <c r="D22" s="55" t="s">
+        <v>724</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="59"/>
+      <c r="B23" s="53"/>
+      <c r="C23" s="13" t="s">
+        <v>722</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="59"/>
+      <c r="B24" s="53"/>
+      <c r="C24" s="13" t="s">
+        <v>723</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>730</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="53" t="s">
+        <v>741</v>
+      </c>
+      <c r="B25" s="53" t="s">
+        <v>731</v>
+      </c>
+      <c r="C25" s="13" t="s">
+        <v>733</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="53"/>
+      <c r="B26" s="53"/>
+      <c r="C26" s="56" t="s">
+        <v>735</v>
+      </c>
+      <c r="D26" s="55" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="53"/>
+      <c r="B27" s="53"/>
+      <c r="C27" s="13" t="s">
+        <v>734</v>
+      </c>
+      <c r="D27" s="13" t="s">
+        <v>736</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="13">
+    <mergeCell ref="A10:A14"/>
+    <mergeCell ref="A15:A20"/>
+    <mergeCell ref="A21:A24"/>
+    <mergeCell ref="A25:A27"/>
+    <mergeCell ref="C5:C9"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B15:B20"/>
+    <mergeCell ref="B21:B24"/>
+    <mergeCell ref="B25:B27"/>
+    <mergeCell ref="A3:A9"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -8677,11 +9253,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H164"/>
+  <dimension ref="A1:H166"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C106" sqref="C106"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A161" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C170" sqref="C170"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8702,7 +9278,7 @@
         <v>63</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>0</v>
+        <v>703</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>343</v>
@@ -8710,90 +9286,90 @@
     </row>
     <row r="2" spans="1:3" s="23" customFormat="1" ht="306.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20"/>
-      <c r="B2" s="41" t="s">
+      <c r="B2" s="47" t="s">
         <v>491</v>
       </c>
       <c r="C2" s="22" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
     </row>
     <row r="3" spans="1:3" s="23" customFormat="1" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A3" s="20"/>
-      <c r="B3" s="42"/>
+      <c r="B3" s="48"/>
       <c r="C3" s="22" t="s">
-        <v>647</v>
+        <v>645</v>
       </c>
     </row>
     <row r="4" spans="1:3" s="23" customFormat="1" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="20"/>
       <c r="B4" s="34" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
       <c r="C4" s="22" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="5" spans="1:3" s="23" customFormat="1" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A5" s="19"/>
       <c r="B5" s="14" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="6" spans="1:3" s="23" customFormat="1" ht="144" x14ac:dyDescent="0.3">
       <c r="A6" s="19"/>
       <c r="B6" s="14" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="7" spans="1:3" s="23" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A7" s="19"/>
       <c r="B7" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
     </row>
     <row r="8" spans="1:3" s="23" customFormat="1" ht="216" x14ac:dyDescent="0.3">
       <c r="A8" s="19"/>
       <c r="B8" s="14" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
     </row>
     <row r="9" spans="1:3" s="23" customFormat="1" ht="216" x14ac:dyDescent="0.3">
       <c r="A9" s="19"/>
       <c r="B9" s="14" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
     </row>
     <row r="10" spans="1:3" s="23" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A10" s="19"/>
       <c r="B10" s="14" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="11" spans="1:3" s="23" customFormat="1" ht="273.60000000000002" x14ac:dyDescent="0.3">
       <c r="A11" s="19"/>
       <c r="B11" s="14" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="12" spans="1:3" s="23" customFormat="1" ht="331.2" x14ac:dyDescent="0.3">
@@ -8802,61 +9378,61 @@
         <v>44</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>661</v>
+        <v>659</v>
       </c>
     </row>
     <row r="13" spans="1:3" s="23" customFormat="1" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A13" s="19"/>
       <c r="B13" s="14" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="14" spans="1:3" s="23" customFormat="1" ht="244.8" x14ac:dyDescent="0.3">
       <c r="A14" s="19"/>
       <c r="B14" s="14" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="15" spans="1:3" s="23" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A15" s="19"/>
       <c r="B15" s="14" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="16" spans="1:3" s="23" customFormat="1" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A16" s="19"/>
       <c r="B16" s="14" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="17" spans="1:4" s="23" customFormat="1" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A17" s="19"/>
       <c r="B17" s="14" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="18" spans="1:4" s="23" customFormat="1" ht="172.8" x14ac:dyDescent="0.3">
       <c r="A18" s="19"/>
       <c r="B18" s="36" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
       <c r="C18" s="14" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
@@ -8864,1085 +9440,1101 @@
         <v>1</v>
       </c>
       <c r="C19" s="14" t="s">
+        <v>580</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B20" s="14" t="s">
+        <v>699</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>700</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B21" s="14" t="s">
+        <v>701</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>702</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="B22" s="14" t="s">
+        <v>654</v>
+      </c>
+      <c r="C22" s="14" t="s">
+        <v>655</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="B23" s="14" t="s">
+        <v>492</v>
+      </c>
+      <c r="C23" s="14" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
+      <c r="B24" s="14" t="s">
+        <v>488</v>
+      </c>
+      <c r="C24" s="14" t="s">
+        <v>581</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="72" x14ac:dyDescent="0.3">
+      <c r="B25" s="14" t="s">
+        <v>674</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
+      <c r="B26" s="11" t="s">
+        <v>433</v>
+      </c>
+      <c r="C26" s="28" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B27" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" s="14" t="s">
+        <v>656</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B28" s="14" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B29" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>497</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B30" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="C30" s="14" t="s">
         <v>582</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B20" s="14" t="s">
-        <v>656</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>657</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="302.39999999999998" x14ac:dyDescent="0.3">
-      <c r="B21" s="14" t="s">
-        <v>492</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>650</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" ht="259.2" x14ac:dyDescent="0.3">
-      <c r="B22" s="14" t="s">
-        <v>488</v>
-      </c>
-      <c r="C22" s="14" t="s">
+      <c r="D30" s="35" t="s">
         <v>583</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="72" x14ac:dyDescent="0.3">
-      <c r="B23" s="14" t="s">
-        <v>680</v>
-      </c>
-      <c r="C23" s="14" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
-      <c r="B24" s="11" t="s">
-        <v>433</v>
-      </c>
-      <c r="C24" s="28" t="s">
-        <v>496</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B25" s="14" t="s">
-        <v>2</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B26" s="14" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B27" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="C27" s="14" t="s">
-        <v>497</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B28" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="C28" s="14" t="s">
-        <v>584</v>
-      </c>
-      <c r="D28" s="35" t="s">
-        <v>585</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B29" s="14" t="s">
-        <v>4</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>449</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="B30" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="C30" s="14" t="s">
-        <v>450</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B31" s="14" t="s">
+        <v>4</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>449</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="B32" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>450</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B33" s="14" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B32" s="14" t="s">
+    <row r="34" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B34" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="14" t="s">
+      <c r="C34" s="14" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="33" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B33" s="14" t="s">
+    <row r="35" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B35" s="14" t="s">
         <v>364</v>
       </c>
-      <c r="C33" s="14" t="s">
+      <c r="C35" s="14" t="s">
         <v>451</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B34" s="14" t="s">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B36" s="14" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="35" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B35" s="14" t="s">
+    <row r="37" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B37" s="14" t="s">
         <v>8</v>
       </c>
-      <c r="C35" s="14" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" s="43"/>
-      <c r="B36" s="44" t="s">
+      <c r="C37" s="14" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" s="38"/>
+      <c r="B38" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="44" t="s">
+      <c r="C38" s="39" t="s">
+        <v>614</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" s="19" customFormat="1" ht="216" x14ac:dyDescent="0.3">
+      <c r="B39" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>615</v>
+      </c>
+      <c r="D39" s="14" t="s">
         <v>616</v>
       </c>
-    </row>
-    <row r="37" spans="1:8" s="19" customFormat="1" ht="216" x14ac:dyDescent="0.3">
-      <c r="B37" s="14" t="s">
-        <v>18</v>
-      </c>
-      <c r="C37" s="14" t="s">
+      <c r="E39" s="14" t="s">
         <v>617</v>
       </c>
-      <c r="D37" s="14" t="s">
+      <c r="F39" s="14" t="s">
         <v>618</v>
       </c>
-      <c r="E37" s="14" t="s">
+      <c r="G39" s="14" t="s">
         <v>619</v>
       </c>
-      <c r="F37" s="14" t="s">
+      <c r="H39" s="14" t="s">
         <v>620</v>
       </c>
-      <c r="G37" s="14" t="s">
+    </row>
+    <row r="40" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A40" s="40"/>
+      <c r="B40" s="41" t="s">
         <v>621</v>
       </c>
-      <c r="H37" s="14" t="s">
+      <c r="C40" s="41" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="72" x14ac:dyDescent="0.3">
+      <c r="B41" s="14" t="s">
         <v>622</v>
       </c>
-    </row>
-    <row r="38" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A38" s="45"/>
-      <c r="B38" s="46" t="s">
+      <c r="C41" s="14" t="s">
         <v>623</v>
       </c>
-      <c r="C38" s="46" t="s">
-        <v>452</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" ht="72" x14ac:dyDescent="0.3">
-      <c r="B39" s="14" t="s">
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B42" s="14" t="s">
         <v>624</v>
       </c>
-      <c r="C39" s="14" t="s">
+      <c r="C42" s="14" t="s">
         <v>625</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B40" s="14" t="s">
-        <v>626</v>
-      </c>
-      <c r="C40" s="14" t="s">
-        <v>627</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B41" s="14" t="s">
-        <v>628</v>
-      </c>
-      <c r="C41" s="14" t="s">
-        <v>629</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B42" s="14" t="s">
-        <v>330</v>
-      </c>
-      <c r="C42" s="14" t="s">
-        <v>630</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.3">
       <c r="B43" s="14" t="s">
-        <v>586</v>
+        <v>626</v>
       </c>
       <c r="C43" s="14" t="s">
+        <v>627</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="B44" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="C44" s="14" t="s">
+        <v>628</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="B45" s="14" t="s">
+        <v>584</v>
+      </c>
+      <c r="C45" s="14" t="s">
         <v>453</v>
       </c>
     </row>
-    <row r="44" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B44" s="14" t="s">
+    <row r="46" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B46" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="14" t="s">
+      <c r="C46" s="14" t="s">
         <v>454</v>
       </c>
     </row>
-    <row r="45" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B45" s="14" t="s">
+    <row r="47" spans="1:8" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B47" s="14" t="s">
         <v>20</v>
       </c>
-      <c r="C45" s="14" t="s">
+      <c r="C47" s="14" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="46" spans="1:8" ht="216" x14ac:dyDescent="0.3">
-      <c r="B46" s="14" t="s">
+    <row r="48" spans="1:8" ht="216" x14ac:dyDescent="0.3">
+      <c r="B48" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="C46" s="14" t="s">
+      <c r="C48" s="14" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="47" spans="1:8" ht="360" x14ac:dyDescent="0.3">
-      <c r="B47" s="14" t="s">
+    <row r="49" spans="2:3" ht="360" x14ac:dyDescent="0.3">
+      <c r="B49" s="14" t="s">
         <v>24</v>
       </c>
-      <c r="C47" s="14" t="s">
+      <c r="C49" s="14" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="48" spans="1:8" ht="100.8" x14ac:dyDescent="0.3">
-      <c r="B48" s="14" t="s">
+    <row r="50" spans="2:3" ht="100.8" x14ac:dyDescent="0.3">
+      <c r="B50" s="14" t="s">
         <v>30</v>
       </c>
-      <c r="C48" s="14" t="s">
-        <v>587</v>
-      </c>
-    </row>
-    <row r="49" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B49" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C49" s="14" t="s">
-        <v>436</v>
-      </c>
-    </row>
-    <row r="50" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B50" s="14" t="s">
-        <v>36</v>
-      </c>
       <c r="C50" s="14" t="s">
-        <v>456</v>
+        <v>585</v>
       </c>
     </row>
     <row r="51" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B51" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C51" s="14" t="s">
+        <v>436</v>
+      </c>
+    </row>
+    <row r="52" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B52" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="C52" s="14" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="53" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B53" s="14" t="s">
         <v>40</v>
       </c>
-      <c r="C51" s="14" t="s">
+      <c r="C53" s="14" t="s">
         <v>457</v>
       </c>
     </row>
-    <row r="52" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B52" s="14" t="s">
+    <row r="54" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B54" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="C52" s="14" t="s">
-        <v>588</v>
-      </c>
-    </row>
-    <row r="53" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B53" s="14" t="s">
+      <c r="C54" s="14" t="s">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="55" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B55" s="14" t="s">
         <v>42</v>
       </c>
-      <c r="C53" s="14" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="54" spans="2:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="B54" s="14" t="s">
+      <c r="C55" s="14" t="s">
+        <v>587</v>
+      </c>
+    </row>
+    <row r="56" spans="2:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B56" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="C54" s="14" t="s">
+      <c r="C56" s="14" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="55" spans="2:3" ht="388.8" x14ac:dyDescent="0.3">
-      <c r="B55" s="14" t="s">
+    <row r="57" spans="2:3" ht="388.8" x14ac:dyDescent="0.3">
+      <c r="B57" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="C55" s="14" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="56" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B56" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="C56" s="14" t="s">
-        <v>438</v>
-      </c>
-    </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B57" s="14" t="s">
-        <v>49</v>
-      </c>
       <c r="C57" s="14" t="s">
-        <v>439</v>
+        <v>676</v>
       </c>
     </row>
     <row r="58" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B58" s="14" t="s">
-        <v>440</v>
+        <v>47</v>
       </c>
       <c r="C58" s="14" t="s">
-        <v>441</v>
+        <v>438</v>
       </c>
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B59" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="C59" s="14" t="s">
+        <v>439</v>
+      </c>
+    </row>
+    <row r="60" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B60" s="14" t="s">
+        <v>440</v>
+      </c>
+      <c r="C60" s="14" t="s">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="61" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B61" s="14" t="s">
         <v>470</v>
       </c>
-      <c r="C59" s="14" t="s">
-        <v>612</v>
-      </c>
-    </row>
-    <row r="60" spans="2:3" ht="216" x14ac:dyDescent="0.3">
-      <c r="B60" s="14" t="s">
+      <c r="C61" s="14" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="62" spans="2:3" ht="216" x14ac:dyDescent="0.3">
+      <c r="B62" s="14" t="s">
         <v>50</v>
       </c>
-      <c r="C60" s="14" t="s">
+      <c r="C62" s="14" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="61" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B61" s="14" t="s">
+    <row r="63" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B63" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="C61" s="14" t="s">
+      <c r="C63" s="14" t="s">
         <v>473</v>
-      </c>
-    </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B62" s="14" t="s">
-        <v>474</v>
-      </c>
-      <c r="C62" s="14" t="s">
-        <v>475</v>
-      </c>
-    </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B63" s="14" t="s">
-        <v>13</v>
-      </c>
-      <c r="C63" s="21" t="s">
-        <v>476</v>
       </c>
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B64" s="14" t="s">
-        <v>14</v>
-      </c>
-      <c r="C64" s="21" t="s">
-        <v>477</v>
+        <v>474</v>
+      </c>
+      <c r="C64" s="14" t="s">
+        <v>475</v>
       </c>
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B65" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C65" s="21" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="66" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B66" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C66" s="21" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="67" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B67" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C65" s="21" t="s">
+      <c r="C67" s="21" t="s">
         <v>478</v>
-      </c>
-    </row>
-    <row r="66" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B66" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C66" s="14" t="s">
-        <v>479</v>
-      </c>
-    </row>
-    <row r="67" spans="2:3" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B67" s="14" t="s">
-        <v>45</v>
-      </c>
-      <c r="C67" s="14" t="s">
-        <v>480</v>
       </c>
     </row>
     <row r="68" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B68" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C68" s="14" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="69" spans="2:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="B69" s="14" t="s">
+        <v>45</v>
+      </c>
+      <c r="C69" s="14" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="70" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B70" s="14" t="s">
+        <v>632</v>
+      </c>
+      <c r="C70" s="14" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="71" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B71" s="14" t="s">
+        <v>51</v>
+      </c>
+      <c r="C71" s="14" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="72" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B72" s="14" t="s">
+        <v>48</v>
+      </c>
+      <c r="C72" s="14" t="s">
         <v>634</v>
       </c>
-      <c r="C68" s="14" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="69" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B69" s="14" t="s">
-        <v>51</v>
-      </c>
-      <c r="C69" s="14" t="s">
-        <v>481</v>
-      </c>
-    </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B70" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="C70" s="14" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="71" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B71" s="14" t="s">
+    </row>
+    <row r="73" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B73" s="14" t="s">
         <v>98</v>
       </c>
-      <c r="C71" s="14" t="s">
+      <c r="C73" s="14" t="s">
         <v>498</v>
       </c>
     </row>
-    <row r="72" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B72" s="14" t="s">
+    <row r="74" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B74" s="14" t="s">
         <v>99</v>
       </c>
-      <c r="C72" s="14" t="s">
+      <c r="C74" s="14" t="s">
         <v>499</v>
       </c>
     </row>
-    <row r="73" spans="2:3" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B73" s="14" t="s">
+    <row r="75" spans="2:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="B75" s="14" t="s">
         <v>100</v>
       </c>
-      <c r="C73" s="14" t="s">
+      <c r="C75" s="14" t="s">
         <v>482</v>
-      </c>
-    </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B74" s="14" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="75" spans="2:3" ht="172.8" x14ac:dyDescent="0.3">
-      <c r="B75" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="C75" s="14" t="s">
-        <v>404</v>
       </c>
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B76" s="14" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="77" spans="2:3" ht="172.8" x14ac:dyDescent="0.3">
+      <c r="B77" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="C77" s="14" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="78" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B78" s="14" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B77" s="14" t="s">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B79" s="14" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="78" spans="2:3" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="B78" s="14" t="s">
+    <row r="80" spans="2:3" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="B80" s="14" t="s">
         <v>122</v>
       </c>
-      <c r="C78" s="14" t="s">
+      <c r="C80" s="14" t="s">
         <v>421</v>
-      </c>
-    </row>
-    <row r="79" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B79" s="14" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B80" s="14" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="81" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B81" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="82" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B82" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="83" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B83" s="14" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="82" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B82" s="14" t="s">
+    <row r="84" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B84" s="14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="83" spans="2:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="B83" s="14" t="s">
+    <row r="85" spans="2:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B85" s="14" t="s">
         <v>512</v>
       </c>
-      <c r="C83" s="14" t="s">
+      <c r="C85" s="14" t="s">
         <v>542</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B84" s="14" t="s">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B86" s="14" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="85" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B85" s="14" t="s">
-        <v>674</v>
-      </c>
-      <c r="C85" s="14" t="s">
-        <v>675</v>
-      </c>
-    </row>
-    <row r="86" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B86" s="14" t="s">
+    <row r="87" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B87" s="14" t="s">
+        <v>668</v>
+      </c>
+      <c r="C87" s="14" t="s">
+        <v>669</v>
+      </c>
+    </row>
+    <row r="88" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B88" s="14" t="s">
         <v>135</v>
-      </c>
-    </row>
-    <row r="87" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B87" s="14" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B88" s="14" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="89" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B89" s="14" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="90" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="90" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B90" s="14" t="s">
-        <v>148</v>
+        <v>137</v>
       </c>
     </row>
     <row r="91" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B91" s="14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="92" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B92" s="14" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="93" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B93" s="14" t="s">
         <v>149</v>
       </c>
-      <c r="C91" s="14" t="s">
+      <c r="C93" s="14" t="s">
         <v>501</v>
       </c>
     </row>
-    <row r="92" spans="2:3" ht="144" x14ac:dyDescent="0.3">
-      <c r="B92" s="14" t="s">
+    <row r="94" spans="2:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="B94" s="14" t="s">
         <v>500</v>
       </c>
-      <c r="C92" s="14" t="s">
-        <v>611</v>
-      </c>
-    </row>
-    <row r="93" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B93" s="14" t="s">
+      <c r="C94" s="14" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="95" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B95" s="14" t="s">
         <v>151</v>
       </c>
-      <c r="C93" s="14" t="s">
+      <c r="C95" s="14" t="s">
         <v>502</v>
       </c>
     </row>
-    <row r="94" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B94" s="14" t="s">
+    <row r="96" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B96" s="14" t="s">
         <v>245</v>
       </c>
-      <c r="C94" s="14" t="s">
+      <c r="C96" s="14" t="s">
         <v>503</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B95" s="14" t="s">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B97" s="14" t="s">
         <v>246</v>
       </c>
-      <c r="C95" s="14" t="s">
+      <c r="C97" s="14" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="96" spans="2:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="B96" s="24" t="s">
+    <row r="98" spans="2:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="B98" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="C96" s="14" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="97" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B97" s="14" t="s">
+      <c r="C98" s="14" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="99" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B99" s="14" t="s">
         <v>248</v>
       </c>
-      <c r="C97" s="14" t="s">
+      <c r="C99" s="14" t="s">
         <v>505</v>
       </c>
     </row>
-    <row r="98" spans="2:3" ht="115.2" x14ac:dyDescent="0.3">
-      <c r="B98" s="14" t="s">
-        <v>632</v>
-      </c>
-      <c r="C98" s="14" t="s">
+    <row r="100" spans="2:3" ht="115.2" x14ac:dyDescent="0.3">
+      <c r="B100" s="14" t="s">
+        <v>630</v>
+      </c>
+      <c r="C100" s="14" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="101" spans="2:3" ht="302.39999999999998" x14ac:dyDescent="0.3">
+      <c r="B101" s="14" t="s">
+        <v>631</v>
+      </c>
+      <c r="C101" s="14" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="102" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B102" s="14" t="s">
+        <v>506</v>
+      </c>
+      <c r="C102" s="14" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="103" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B103" s="14" t="s">
+        <v>249</v>
+      </c>
+      <c r="C103" s="14" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="104" spans="2:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="B104" s="14" t="s">
+        <v>250</v>
+      </c>
+      <c r="C104" s="14" t="s">
+        <v>507</v>
+      </c>
+    </row>
+    <row r="105" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B105" s="14" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="106" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B106" s="14" t="s">
+        <v>252</v>
+      </c>
+      <c r="C106" s="14" t="s">
+        <v>423</v>
+      </c>
+    </row>
+    <row r="107" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B107" s="14" t="s">
+        <v>508</v>
+      </c>
+      <c r="C107" s="14" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="108" spans="2:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="B108" s="14" t="s">
+        <v>510</v>
+      </c>
+      <c r="C108" s="14" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="109" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B109" s="14" t="s">
+        <v>253</v>
+      </c>
+      <c r="C109" s="14" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="110" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B110" s="14" t="s">
+        <v>254</v>
+      </c>
+      <c r="C110" s="14" t="s">
         <v>637</v>
-      </c>
-    </row>
-    <row r="99" spans="2:3" ht="302.39999999999998" x14ac:dyDescent="0.3">
-      <c r="B99" s="14" t="s">
-        <v>633</v>
-      </c>
-      <c r="C99" s="14" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="100" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B100" s="14" t="s">
-        <v>506</v>
-      </c>
-      <c r="C100" s="14" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="101" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B101" s="14" t="s">
-        <v>249</v>
-      </c>
-      <c r="C101" s="14" t="s">
-        <v>631</v>
-      </c>
-    </row>
-    <row r="102" spans="2:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="B102" s="14" t="s">
-        <v>250</v>
-      </c>
-      <c r="C102" s="14" t="s">
-        <v>507</v>
-      </c>
-    </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B103" s="14" t="s">
-        <v>251</v>
-      </c>
-    </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B104" s="14" t="s">
-        <v>252</v>
-      </c>
-      <c r="C104" s="14" t="s">
-        <v>423</v>
-      </c>
-    </row>
-    <row r="105" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B105" s="14" t="s">
-        <v>508</v>
-      </c>
-      <c r="C105" s="14" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="106" spans="2:3" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="B106" s="14" t="s">
-        <v>510</v>
-      </c>
-      <c r="C106" s="14" t="s">
-        <v>684</v>
-      </c>
-    </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B107" s="14" t="s">
-        <v>253</v>
-      </c>
-      <c r="C107" s="14" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="108" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B108" s="14" t="s">
-        <v>254</v>
-      </c>
-      <c r="C108" s="14" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="109" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B109" s="14" t="s">
-        <v>255</v>
-      </c>
-      <c r="C109" s="21" t="s">
-        <v>511</v>
-      </c>
-    </row>
-    <row r="110" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B110" s="14" t="s">
-        <v>256</v>
-      </c>
-      <c r="C110" s="14" t="s">
-        <v>427</v>
       </c>
     </row>
     <row r="111" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B111" s="14" t="s">
-        <v>257</v>
-      </c>
-      <c r="C111" s="14" t="s">
-        <v>428</v>
+        <v>255</v>
+      </c>
+      <c r="C111" s="21" t="s">
+        <v>511</v>
       </c>
     </row>
     <row r="112" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B112" s="14" t="s">
+        <v>256</v>
+      </c>
+      <c r="C112" s="14" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="113" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B113" s="14" t="s">
+        <v>257</v>
+      </c>
+      <c r="C113" s="14" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="114" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B114" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="C112" s="14" t="s">
+      <c r="C114" s="14" t="s">
         <v>429</v>
-      </c>
-    </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B113" s="14" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B114" s="14" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B115" s="14" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="116" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B116" s="14" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="117" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B117" s="14" t="s">
         <v>261</v>
       </c>
-      <c r="C115" s="14" t="s">
+      <c r="C117" s="14" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="118" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B118" s="14" t="s">
+        <v>262</v>
+      </c>
+      <c r="C118" s="14" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="119" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B119" s="14" t="s">
+        <v>263</v>
+      </c>
+      <c r="C119" s="14" t="s">
         <v>640</v>
       </c>
     </row>
-    <row r="116" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B116" s="14" t="s">
-        <v>262</v>
-      </c>
-      <c r="C116" s="14" t="s">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B120" s="14" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="121" spans="2:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="B121" s="14" t="s">
+        <v>265</v>
+      </c>
+      <c r="C121" s="14" t="s">
         <v>641</v>
-      </c>
-    </row>
-    <row r="117" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B117" s="14" t="s">
-        <v>263</v>
-      </c>
-      <c r="C117" s="14" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B118" s="14" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="119" spans="2:3" ht="72" x14ac:dyDescent="0.3">
-      <c r="B119" s="14" t="s">
-        <v>265</v>
-      </c>
-      <c r="C119" s="14" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="120" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="B120" s="14" t="s">
-        <v>266</v>
-      </c>
-      <c r="C120" s="14" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B121" s="14" t="s">
-        <v>267</v>
       </c>
     </row>
     <row r="122" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B122" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="C122" s="14" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="123" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B123" s="14" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="124" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="B124" s="14" t="s">
         <v>268</v>
       </c>
-      <c r="C122" s="14" t="s">
+      <c r="C124" s="14" t="s">
         <v>459</v>
       </c>
     </row>
-    <row r="123" spans="2:3" ht="374.4" x14ac:dyDescent="0.3">
-      <c r="B123" s="14" t="s">
+    <row r="125" spans="2:3" ht="374.4" x14ac:dyDescent="0.3">
+      <c r="B125" s="14" t="s">
         <v>269</v>
       </c>
-      <c r="C123" s="14" t="s">
+      <c r="C125" s="14" t="s">
         <v>458</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B124" s="14" t="s">
+    <row r="126" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B126" s="14" t="s">
         <v>270</v>
       </c>
-      <c r="C124" s="14" t="s">
+      <c r="C126" s="14" t="s">
         <v>460</v>
-      </c>
-    </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B125" s="14" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="126" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B126" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="C126" s="14" t="s">
-        <v>461</v>
       </c>
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B127" s="14" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="128" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B128" s="14" t="s">
+        <v>272</v>
+      </c>
+      <c r="C128" s="14" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="129" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B129" s="14" t="s">
         <v>273</v>
-      </c>
-    </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B128" s="14" t="s">
-        <v>274</v>
-      </c>
-    </row>
-    <row r="129" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B129" s="14" t="s">
-        <v>275</v>
       </c>
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B130" s="14" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="131" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B131" s="14" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="132" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B132" s="14" t="s">
         <v>276</v>
-      </c>
-    </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B131" s="14" t="s">
-        <v>277</v>
-      </c>
-    </row>
-    <row r="132" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B132" s="14" t="s">
-        <v>677</v>
-      </c>
-      <c r="C132" s="14" t="s">
-        <v>678</v>
       </c>
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B133" s="14" t="s">
-        <v>278</v>
-      </c>
-    </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.3">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="134" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B134" s="14" t="s">
-        <v>279</v>
+        <v>671</v>
       </c>
       <c r="C134" s="14" t="s">
-        <v>462</v>
+        <v>672</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B135" s="14" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B136" s="14" t="s">
-        <v>281</v>
+        <v>279</v>
+      </c>
+      <c r="C136" s="14" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B137" s="14" t="s">
-        <v>282</v>
+        <v>280</v>
       </c>
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B138" s="14" t="s">
-        <v>329</v>
+        <v>281</v>
       </c>
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B139" s="14" t="s">
-        <v>330</v>
-      </c>
-    </row>
-    <row r="140" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="140" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B140" s="14" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B141" s="14" t="s">
-        <v>332</v>
-      </c>
-    </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.3">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="142" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B142" s="14" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B143" s="14" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="144" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B144" s="14" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="145" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B145" s="14" t="s">
         <v>334</v>
       </c>
     </row>
-    <row r="144" spans="2:3" ht="86.4" x14ac:dyDescent="0.3">
-      <c r="B144" s="14" t="s">
+    <row r="146" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="B146" s="14" t="s">
         <v>335</v>
       </c>
-      <c r="C144" s="14" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="145" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B145" s="14" t="s">
+      <c r="C146" s="14" t="s">
+        <v>670</v>
+      </c>
+    </row>
+    <row r="147" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B147" s="14" t="s">
         <v>336</v>
       </c>
-      <c r="C145" s="14" t="s">
-        <v>673</v>
-      </c>
-    </row>
-    <row r="146" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B146" s="14" t="s">
+      <c r="C147" s="14" t="s">
+        <v>667</v>
+      </c>
+    </row>
+    <row r="148" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B148" s="14" t="s">
         <v>387</v>
       </c>
-      <c r="C146" s="14" t="s">
+      <c r="C148" s="14" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147" s="20"/>
-      <c r="B147" s="14" t="s">
-        <v>392</v>
-      </c>
-    </row>
-    <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" s="20"/>
-      <c r="B148" s="14" t="s">
-        <v>659</v>
-      </c>
-      <c r="C148" s="14" t="s">
-        <v>660</v>
-      </c>
-    </row>
-    <row r="149" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="20"/>
       <c r="B149" s="14" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A150" s="20"/>
+      <c r="B150" s="14" t="s">
+        <v>657</v>
+      </c>
+      <c r="C150" s="14" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="151" spans="1:3" ht="86.4" x14ac:dyDescent="0.3">
+      <c r="A151" s="20"/>
+      <c r="B151" s="14" t="s">
         <v>399</v>
       </c>
-      <c r="C149" s="14" t="s">
+      <c r="C151" s="14" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="150" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A150" s="38" t="s">
+    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A152" s="44" t="s">
         <v>472</v>
       </c>
-      <c r="B150" s="39"/>
-      <c r="C150" s="40"/>
-    </row>
-    <row r="151" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B151" s="14" t="s">
+      <c r="B152" s="45"/>
+      <c r="C152" s="46"/>
+    </row>
+    <row r="153" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B153" s="14" t="s">
         <v>405</v>
       </c>
-      <c r="C151" s="14" t="s">
+      <c r="C153" s="14" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="152" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B152" s="14" t="s">
+    <row r="154" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B154" s="14" t="s">
         <v>407</v>
       </c>
-      <c r="C152" s="14" t="s">
+      <c r="C154" s="14" t="s">
         <v>408</v>
-      </c>
-    </row>
-    <row r="153" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B153" s="14" t="s">
-        <v>409</v>
-      </c>
-      <c r="C153" s="14" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B154" s="14" t="s">
-        <v>411</v>
-      </c>
-      <c r="C154" s="14" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B155" s="14" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="C155" s="14" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B156" s="14" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="C156" s="14" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
       <c r="B157" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="C157" s="14" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B158" s="14" t="s">
+        <v>415</v>
+      </c>
+      <c r="C158" s="14" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="B159" s="14" t="s">
         <v>417</v>
       </c>
-      <c r="C157" s="14" t="s">
+      <c r="C159" s="14" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="158" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B158" s="14" t="s">
+    <row r="160" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="B160" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C158" s="14" t="s">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="C159" s="14" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" ht="144" x14ac:dyDescent="0.3">
-      <c r="B160" s="14" t="s">
+      <c r="C160" s="14" t="s">
+        <v>664</v>
+      </c>
+    </row>
+    <row r="161" spans="2:3" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="C161" s="14" t="s">
+        <v>660</v>
+      </c>
+    </row>
+    <row r="162" spans="2:3" ht="144" x14ac:dyDescent="0.3">
+      <c r="B162" s="14" t="s">
+        <v>661</v>
+      </c>
+      <c r="C162" s="14" t="s">
         <v>663</v>
       </c>
-      <c r="C160" s="14" t="s">
-        <v>669</v>
-      </c>
-    </row>
-    <row r="161" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B161" s="14" t="s">
+    </row>
+    <row r="163" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="B163" s="14" t="s">
         <v>419</v>
       </c>
-      <c r="C161" s="14" t="s">
+      <c r="C163" s="14" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="162" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B162" s="14" t="s">
+    <row r="164" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B164" s="14" t="s">
         <v>425</v>
       </c>
-      <c r="C162" s="14" t="s">
+      <c r="C164" s="14" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B163" s="14" t="s">
+    <row r="165" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B165" s="14" t="s">
         <v>484</v>
       </c>
-      <c r="C163" s="14" t="s">
+      <c r="C165" s="14" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.3">
-      <c r="B164" s="14" t="s">
+    <row r="166" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B166" s="14" t="s">
         <v>485</v>
       </c>
-      <c r="C164" s="14" t="s">
+      <c r="C166" s="14" t="s">
         <v>487</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A150:C150"/>
+    <mergeCell ref="A152:C152"/>
     <mergeCell ref="B2:B3"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C63" r:id="rId1" location=":~:text=WeakHashMap%20is%20an%20implementation%20of,Garbage%20Collector%20dominates%20over%20WeakHashMap." xr:uid="{8DF82765-60D3-449F-AD2D-19DD872E3BA6}"/>
-    <hyperlink ref="C64" r:id="rId2" xr:uid="{99F4FBAD-904D-4F81-8F65-67E23FAD25F1}"/>
-    <hyperlink ref="C65" r:id="rId3" xr:uid="{35A27C47-788D-4C68-97AC-FC16766F27C7}"/>
-    <hyperlink ref="C109" r:id="rId4" xr:uid="{3F17D884-C7A9-4AD8-952F-91D16B01C812}"/>
-    <hyperlink ref="D28" r:id="rId5" xr:uid="{DCE73648-524B-46C4-8889-34B6E79B566D}"/>
+    <hyperlink ref="C65" r:id="rId1" location=":~:text=WeakHashMap%20is%20an%20implementation%20of,Garbage%20Collector%20dominates%20over%20WeakHashMap." xr:uid="{8DF82765-60D3-449F-AD2D-19DD872E3BA6}"/>
+    <hyperlink ref="C66" r:id="rId2" xr:uid="{99F4FBAD-904D-4F81-8F65-67E23FAD25F1}"/>
+    <hyperlink ref="C67" r:id="rId3" xr:uid="{35A27C47-788D-4C68-97AC-FC16766F27C7}"/>
+    <hyperlink ref="C111" r:id="rId4" xr:uid="{3F17D884-C7A9-4AD8-952F-91D16B01C812}"/>
+    <hyperlink ref="D30" r:id="rId5" xr:uid="{DCE73648-524B-46C4-8889-34B6E79B566D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId6"/>
@@ -9953,7 +10545,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51032E14-0A5D-4151-8C06-445604791B52}">
   <dimension ref="A1:B64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
+    <sheetView topLeftCell="A29" workbookViewId="0">
       <selection activeCell="A49" sqref="A49:B64"/>
     </sheetView>
   </sheetViews>
@@ -9965,111 +10557,111 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A1" s="47" t="s">
-        <v>575</v>
+      <c r="A1" s="42" t="s">
+        <v>573</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="86.4" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
+        <v>575</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>576</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="49" t="s">
+        <v>570</v>
+      </c>
+      <c r="B6" s="10" t="s">
         <v>577</v>
       </c>
-      <c r="B2" s="11" t="s">
-        <v>578</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="48" t="s">
-        <v>572</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>579</v>
-      </c>
     </row>
     <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="48"/>
+      <c r="A7" s="49"/>
       <c r="B7" s="11" t="s">
-        <v>688</v>
+        <v>681</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="48"/>
-      <c r="B8" s="49" t="s">
-        <v>703</v>
+      <c r="A8" s="49"/>
+      <c r="B8" s="43" t="s">
+        <v>696</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="48"/>
+      <c r="A9" s="49"/>
       <c r="B9" s="11" t="s">
-        <v>693</v>
+        <v>686</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="48"/>
+      <c r="A10" s="49"/>
       <c r="B10" s="11"/>
     </row>
     <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="48"/>
+      <c r="A11" s="49"/>
       <c r="B11" s="11" t="s">
-        <v>685</v>
+        <v>678</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="48"/>
+      <c r="A12" s="49"/>
       <c r="B12" s="10" t="s">
-        <v>686</v>
+        <v>679</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="48"/>
+      <c r="A13" s="49"/>
       <c r="B13" s="10"/>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="48"/>
+      <c r="A14" s="49"/>
       <c r="B14" s="10" t="s">
-        <v>687</v>
+        <v>680</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="48"/>
+      <c r="A15" s="49"/>
       <c r="B15" s="10"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="48"/>
+      <c r="A16" s="49"/>
       <c r="B16" s="11"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="48"/>
+      <c r="A17" s="49"/>
       <c r="B17" s="10"/>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="48"/>
+      <c r="A18" s="49"/>
       <c r="B18" s="10"/>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="48"/>
+      <c r="A19" s="49"/>
       <c r="B19" s="10"/>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="48"/>
+      <c r="A20" s="49"/>
       <c r="B20" s="10"/>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="48"/>
+      <c r="A21" s="49"/>
       <c r="B21" s="10"/>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="48"/>
+      <c r="A22" s="49"/>
       <c r="B22" s="10"/>
     </row>
     <row r="24" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A24" s="50" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
       <c r="B24" s="11" t="s">
-        <v>689</v>
+        <v>682</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -10083,7 +10675,7 @@
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27" s="50"/>
       <c r="B27" s="10" t="s">
-        <v>692</v>
+        <v>685</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -10097,7 +10689,7 @@
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A30" s="50"/>
       <c r="B30" s="10" t="s">
-        <v>690</v>
+        <v>683</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -10111,7 +10703,7 @@
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A33" s="50"/>
       <c r="B33" s="10" t="s">
-        <v>691</v>
+        <v>684</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -10125,7 +10717,7 @@
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A36" s="50"/>
       <c r="B36" s="10" t="s">
-        <v>694</v>
+        <v>687</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -10139,7 +10731,7 @@
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A39" s="50"/>
       <c r="B39" s="10" t="s">
-        <v>695</v>
+        <v>688</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -10153,7 +10745,7 @@
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A42" s="50"/>
       <c r="B42" s="10" t="s">
-        <v>696</v>
+        <v>689</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -10167,7 +10759,7 @@
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A45" s="50"/>
       <c r="B45" s="10" t="s">
-        <v>697</v>
+        <v>690</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -10179,81 +10771,81 @@
       <c r="B47" s="10"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="48" t="s">
-        <v>574</v>
+      <c r="A49" s="49" t="s">
+        <v>572</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="48"/>
+      <c r="A50" s="49"/>
       <c r="B50" s="10"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="48"/>
+      <c r="A51" s="49"/>
       <c r="B51" s="10" t="s">
-        <v>698</v>
+        <v>691</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="48"/>
+      <c r="A52" s="49"/>
       <c r="B52" s="10"/>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="48"/>
+      <c r="A53" s="49"/>
       <c r="B53" s="10"/>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="48"/>
+      <c r="A54" s="49"/>
       <c r="B54" s="10" t="s">
-        <v>700</v>
+        <v>693</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="48"/>
+      <c r="A55" s="49"/>
       <c r="B55" s="10"/>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="48"/>
+      <c r="A56" s="49"/>
       <c r="B56" s="10"/>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="48"/>
+      <c r="A57" s="49"/>
       <c r="B57" s="10" t="s">
-        <v>699</v>
+        <v>692</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="48"/>
+      <c r="A58" s="49"/>
       <c r="B58" s="10"/>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="48"/>
+      <c r="A59" s="49"/>
       <c r="B59" s="10"/>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="48"/>
+      <c r="A60" s="49"/>
       <c r="B60" s="10" t="s">
-        <v>701</v>
+        <v>694</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="48"/>
+      <c r="A61" s="49"/>
       <c r="B61" s="10"/>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="48"/>
+      <c r="A62" s="49"/>
       <c r="B62" s="10"/>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="48"/>
+      <c r="A63" s="49"/>
       <c r="B63" s="10" t="s">
-        <v>702</v>
+        <v>695</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="48"/>
+      <c r="A64" s="49"/>
       <c r="B64" s="10"/>
     </row>
   </sheetData>
@@ -10430,7 +11022,7 @@
         <v>174</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>679</v>
+        <v>673</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -11051,7 +11643,7 @@
         <v>283</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>668</v>
+        <v>662</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
created a separate sheet for java-8
</commit_message>
<xml_diff>
--- a/TechStack.xlsx
+++ b/TechStack.xlsx
@@ -3,26 +3,27 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19EE7FAC-64FE-4DE5-8433-E6E5A91FD275}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3055FD94-5CEC-42C4-8FBF-38FAC910A414}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="979" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="979" firstSheet="2" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SDLC" sheetId="17" r:id="rId1"/>
     <sheet name="Solid Principles" sheetId="19" r:id="rId2"/>
     <sheet name="Core Java" sheetId="1" r:id="rId3"/>
-    <sheet name="Design Patterns" sheetId="18" r:id="rId4"/>
-    <sheet name="Spring" sheetId="2" r:id="rId5"/>
-    <sheet name="Hibernate" sheetId="3" r:id="rId6"/>
-    <sheet name="WebServices" sheetId="5" r:id="rId7"/>
-    <sheet name="Microservices" sheetId="14" r:id="rId8"/>
-    <sheet name="Apache Camel" sheetId="11" r:id="rId9"/>
-    <sheet name="Angular Js" sheetId="12" r:id="rId10"/>
-    <sheet name="SystemDesign" sheetId="16" r:id="rId11"/>
-    <sheet name="SQL" sheetId="4" r:id="rId12"/>
-    <sheet name="Programs" sheetId="6" r:id="rId13"/>
-    <sheet name="Project &amp; Others" sheetId="9" r:id="rId14"/>
-    <sheet name="Learning Material" sheetId="10" r:id="rId15"/>
+    <sheet name="java8" sheetId="20" r:id="rId4"/>
+    <sheet name="Design Patterns" sheetId="18" r:id="rId5"/>
+    <sheet name="Spring" sheetId="2" r:id="rId6"/>
+    <sheet name="Hibernate" sheetId="3" r:id="rId7"/>
+    <sheet name="WebServices" sheetId="5" r:id="rId8"/>
+    <sheet name="Microservices" sheetId="14" r:id="rId9"/>
+    <sheet name="Apache Camel" sheetId="11" r:id="rId10"/>
+    <sheet name="Angular Js" sheetId="12" r:id="rId11"/>
+    <sheet name="SystemDesign" sheetId="16" r:id="rId12"/>
+    <sheet name="SQL" sheetId="4" r:id="rId13"/>
+    <sheet name="Programs" sheetId="6" r:id="rId14"/>
+    <sheet name="Project &amp; Others" sheetId="9" r:id="rId15"/>
+    <sheet name="Learning Material" sheetId="10" r:id="rId16"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="793" uniqueCount="744">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="744">
   <si>
     <t>Topic</t>
   </si>
@@ -5475,247 +5476,6 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>a)</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> Functional Programming</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-b) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Lambda expressions</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-c) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Streams API</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (Streams are sequence of objects that supports various methods to acheive a desired result)
-Ex: 
-list.stream().map().collect(collector.toList());
-list.stream().filter().collect(collector.toList());
-list.stream().sorted().collect(collector.toList());
-Stream is a process of creation of the stream, perform operations on the stream and Consume the result
-d) In java 8 we can define the methods in the interfaces, they were introduced to provide backward compatibility.(i.e) it will not affect the existing code which was written in java 6/java 7
-we can define </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>default</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> and </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>static</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> methods
-interface I{
-  void add();
-    </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>default</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> void show(){
-    define the methods in the interface.
-  }
-  </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>static</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> void display(){
-  }
-}
-e) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>Method Reference</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-Method reference is used to refer method of functional interface. It is compact and easy form of lambda expression. Each time when you are using lambda expression to just referring a method, you can replace your lambda expression with method reference.
-(o) -&gt; o.toString(); (Lambda expression)
-Object::toString(); (Instead of lambda expression, we can make use of the method reference)
-Below are the types of the method references available as part of the java-8
-    i) Instance method reference
-   ii) Static method reference String::</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>valueOf</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-  iii) Constructor reference
-f) </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <u/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Optional classes: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> it is wrapper class used for expressing optionality.</t>
-    </r>
-  </si>
-  <si>
     <t>System Design interview questions</t>
   </si>
   <si>
@@ -6322,6 +6082,268 @@
   </si>
   <si>
     <t>Can we start a thread without a run method?</t>
+  </si>
+  <si>
+    <r>
+      <t>a)</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Functional Programming</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+b) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Lambda expressions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+c) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Streams API</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> (Streams are sequence of objects that supports various methods to acheive a desired result)
+Ex: 
+list.stream().map(Function&lt;&gt;).collect(collector.toList());
+list.stream().filter(Pridicate&lt;&gt;).collect(collector.toList());
+list.stream().sorted().collect(collector.toList());
+Stream is a process of creation of the stream, perform operations on the stream and Consume the result
+d) In java 8 we can define the methods in the interfaces, they were introduced to provide backward compatibility.(i.e) it will not affect the existing code which was written in java 6/java 7
+we can define </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>default</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>static</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> methods
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>@FunctionalInterface</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+interface I{
+    void add();  // Single Abstract Method
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>default</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> void show(){ // default method introduced as part of java-8
+         define the methods in the interface.
+    }
+    </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>static</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> void display(){  // static methods introduced as part of java 8
+   }
+}
+e) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Method Reference</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+Method reference is used to refer method of functional interface. It is compact and easy form of lambda expression. Each time when you are using lambda expression to just referring a method, you can replace your lambda expression with method reference.
+(o) -&gt; o.toString(); (Lambda expression)
+Object::toString(); (Instead of lambda expression, we can make use of the method reference)
+Below are the types of the method references available as part of the java-8
+    i) Instance method reference
+   ii) Static method reference String::</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>valueOf</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+  iii) Constructor reference
+f) </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Optional classes: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> it is wrapper class used for expressing optionality.</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -6614,7 +6636,7 @@
     <xf numFmtId="0" fontId="18" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
@@ -6747,25 +6769,16 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -6778,6 +6791,21 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="2" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="4" xfId="2" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -7356,7 +7384,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6ADC389A-9F0E-41B8-8C1E-C0071BC3B5C1}">
   <dimension ref="A1:D8"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A276" workbookViewId="0">
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
@@ -7383,7 +7411,7 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B3" s="31" t="s">
-        <v>695</v>
+        <v>694</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -7403,7 +7431,7 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B7" s="31" t="s">
-        <v>696</v>
+        <v>695</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
@@ -7419,6 +7447,45 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8385B5A8-9213-481B-8B93-B8B0D707D64F}">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="28.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="12" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>394</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BE406AE7-19D9-4DA9-84B5-63D1C585050C}">
   <dimension ref="A1:C4"/>
   <sheetViews>
@@ -7470,7 +7537,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E0F11CA-2C1E-4DAF-B653-8508FE8E9354}">
   <dimension ref="B1:B11"/>
   <sheetViews>
@@ -7510,12 +7577,12 @@
     </row>
     <row r="10" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
-        <v>663</v>
+        <v>662</v>
       </c>
     </row>
     <row r="11" spans="2:2" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
-        <v>664</v>
+        <v>663</v>
       </c>
     </row>
   </sheetData>
@@ -7524,7 +7591,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:D21"/>
   <sheetViews>
@@ -7682,7 +7749,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:C52"/>
   <sheetViews>
@@ -8036,7 +8103,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C63"/>
   <sheetViews>
@@ -8631,7 +8698,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:C33"/>
   <sheetViews>
@@ -9002,244 +9069,239 @@
     <row r="2" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A2" s="47"/>
       <c r="B2" s="48" t="s">
+        <v>701</v>
+      </c>
+      <c r="C2" s="13" t="s">
         <v>702</v>
       </c>
-      <c r="C2" s="13" t="s">
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="51" t="s">
+        <v>734</v>
+      </c>
+      <c r="B3" s="51" t="s">
         <v>703</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="49" t="s">
+      <c r="C3" s="9" t="s">
+        <v>704</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="51"/>
+      <c r="B4" s="51"/>
+      <c r="C4" s="44" t="s">
+        <v>723</v>
+      </c>
+      <c r="D4" s="45" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="51"/>
+      <c r="B5" s="51"/>
+      <c r="C5" s="49" t="s">
+        <v>722</v>
+      </c>
+      <c r="D5" s="49" t="s">
+        <v>706</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="51"/>
+      <c r="B6" s="51"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+    </row>
+    <row r="7" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="51"/>
+      <c r="B7" s="51"/>
+      <c r="C7" s="50"/>
+      <c r="D7" s="50"/>
+    </row>
+    <row r="8" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="51"/>
+      <c r="B8" s="51"/>
+      <c r="C8" s="50"/>
+      <c r="D8" s="13" t="s">
+        <v>707</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="51"/>
+      <c r="B9" s="51"/>
+      <c r="C9" s="50"/>
+      <c r="D9" s="13" t="s">
+        <v>708</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10" s="51" t="s">
         <v>735</v>
       </c>
-      <c r="B3" s="49" t="s">
-        <v>704</v>
-      </c>
-      <c r="C3" s="9" t="s">
+      <c r="B10" s="51" t="s">
+        <v>709</v>
+      </c>
+      <c r="C10" s="9" t="s">
+        <v>710</v>
+      </c>
+      <c r="D10" s="45" t="s">
         <v>705</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="49"/>
-      <c r="B4" s="49"/>
-      <c r="C4" s="44" t="s">
+    <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A11" s="51"/>
+      <c r="B11" s="51"/>
+      <c r="C11" s="49" t="s">
         <v>724</v>
       </c>
-      <c r="D4" s="45" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="49"/>
-      <c r="B5" s="49"/>
-      <c r="C5" s="51" t="s">
-        <v>723</v>
-      </c>
-      <c r="D5" s="51" t="s">
-        <v>707</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="49"/>
-      <c r="B6" s="49"/>
-      <c r="C6" s="52"/>
-      <c r="D6" s="52"/>
-    </row>
-    <row r="7" spans="1:4" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="49"/>
-      <c r="B7" s="49"/>
-      <c r="C7" s="52"/>
-      <c r="D7" s="52"/>
-    </row>
-    <row r="8" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="49"/>
-      <c r="B8" s="49"/>
-      <c r="C8" s="52"/>
-      <c r="D8" s="13" t="s">
-        <v>708</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="49"/>
-      <c r="B9" s="49"/>
-      <c r="C9" s="52"/>
-      <c r="D9" s="13" t="s">
-        <v>709</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="49" t="s">
+      <c r="D11" s="13" t="s">
+        <v>711</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="51"/>
+      <c r="B12" s="51"/>
+      <c r="C12" s="50"/>
+      <c r="D12" s="13" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="51"/>
+      <c r="B13" s="51"/>
+      <c r="C13" s="50"/>
+      <c r="D13" s="13" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A14" s="51"/>
+      <c r="B14" s="51"/>
+      <c r="C14" s="50"/>
+      <c r="D14" s="13" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A15" s="51" t="s">
         <v>736</v>
       </c>
-      <c r="B10" s="49" t="s">
-        <v>710</v>
-      </c>
-      <c r="C10" s="9" t="s">
+      <c r="B15" s="51" t="s">
+        <v>715</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>729</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A16" s="51"/>
+      <c r="B16" s="51"/>
+      <c r="C16" s="13" t="s">
         <v>711</v>
       </c>
-      <c r="D10" s="45" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A11" s="49"/>
-      <c r="B11" s="49"/>
-      <c r="C11" s="51" t="s">
+    </row>
+    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A17" s="51"/>
+      <c r="B17" s="51"/>
+      <c r="C17" s="13" t="s">
+        <v>712</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A18" s="51"/>
+      <c r="B18" s="51"/>
+      <c r="C18" s="13" t="s">
+        <v>713</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="51"/>
+      <c r="B19" s="51"/>
+      <c r="C19" s="13" t="s">
+        <v>714</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="51"/>
+      <c r="B20" s="51"/>
+      <c r="C20" s="13" t="s">
+        <v>716</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A21" s="52" t="s">
+        <v>737</v>
+      </c>
+      <c r="B21" s="51" t="s">
+        <v>717</v>
+      </c>
+      <c r="C21" s="13" t="s">
+        <v>718</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A22" s="52"/>
+      <c r="B22" s="51"/>
+      <c r="C22" s="44" t="s">
         <v>725</v>
       </c>
-      <c r="D11" s="13" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="49"/>
-      <c r="B12" s="49"/>
-      <c r="C12" s="52"/>
-      <c r="D12" s="13" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="49"/>
-      <c r="B13" s="49"/>
-      <c r="C13" s="52"/>
-      <c r="D13" s="13" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="49"/>
-      <c r="B14" s="49"/>
-      <c r="C14" s="52"/>
-      <c r="D14" s="13" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A15" s="49" t="s">
-        <v>737</v>
-      </c>
-      <c r="B15" s="49" t="s">
-        <v>716</v>
-      </c>
-      <c r="C15" s="13" t="s">
+      <c r="D22" s="45" t="s">
+        <v>721</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="52"/>
+      <c r="B23" s="51"/>
+      <c r="C23" s="13" t="s">
+        <v>719</v>
+      </c>
+      <c r="D23" s="13" t="s">
+        <v>726</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A24" s="52"/>
+      <c r="B24" s="51"/>
+      <c r="C24" s="13" t="s">
+        <v>720</v>
+      </c>
+      <c r="D24" s="13" t="s">
+        <v>727</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A25" s="51" t="s">
+        <v>738</v>
+      </c>
+      <c r="B25" s="51" t="s">
+        <v>728</v>
+      </c>
+      <c r="C25" s="13" t="s">
         <v>730</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A16" s="49"/>
-      <c r="B16" s="49"/>
-      <c r="C16" s="13" t="s">
-        <v>712</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A17" s="49"/>
-      <c r="B17" s="49"/>
-      <c r="C17" s="13" t="s">
-        <v>713</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="49"/>
-      <c r="B18" s="49"/>
-      <c r="C18" s="13" t="s">
-        <v>714</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="49"/>
-      <c r="B19" s="49"/>
-      <c r="C19" s="13" t="s">
-        <v>715</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="49"/>
-      <c r="B20" s="49"/>
-      <c r="C20" s="13" t="s">
-        <v>717</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A21" s="50" t="s">
-        <v>738</v>
-      </c>
-      <c r="B21" s="49" t="s">
-        <v>718</v>
-      </c>
-      <c r="C21" s="13" t="s">
-        <v>719</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A22" s="50"/>
-      <c r="B22" s="49"/>
-      <c r="C22" s="44" t="s">
-        <v>726</v>
-      </c>
-      <c r="D22" s="45" t="s">
-        <v>722</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="50"/>
-      <c r="B23" s="49"/>
-      <c r="C23" s="13" t="s">
-        <v>720</v>
-      </c>
-      <c r="D23" s="13" t="s">
-        <v>727</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A24" s="50"/>
-      <c r="B24" s="49"/>
-      <c r="C24" s="13" t="s">
-        <v>721</v>
-      </c>
-      <c r="D24" s="13" t="s">
-        <v>728</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A25" s="49" t="s">
-        <v>739</v>
-      </c>
-      <c r="B25" s="49" t="s">
-        <v>729</v>
-      </c>
-      <c r="C25" s="13" t="s">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A26" s="51"/>
+      <c r="B26" s="51"/>
+      <c r="C26" s="46" t="s">
+        <v>732</v>
+      </c>
+      <c r="D26" s="45" t="s">
+        <v>705</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
+      <c r="A27" s="51"/>
+      <c r="B27" s="51"/>
+      <c r="C27" s="13" t="s">
         <v>731</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A26" s="49"/>
-      <c r="B26" s="49"/>
-      <c r="C26" s="46" t="s">
+      <c r="D27" s="13" t="s">
         <v>733</v>
-      </c>
-      <c r="D26" s="45" t="s">
-        <v>706</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A27" s="49"/>
-      <c r="B27" s="49"/>
-      <c r="C27" s="13" t="s">
-        <v>732</v>
-      </c>
-      <c r="D27" s="13" t="s">
-        <v>734</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="D5:D7"/>
-    <mergeCell ref="B3:B9"/>
-    <mergeCell ref="C11:C14"/>
-    <mergeCell ref="B10:B14"/>
-    <mergeCell ref="B15:B20"/>
     <mergeCell ref="A10:A14"/>
     <mergeCell ref="A15:A20"/>
     <mergeCell ref="A21:A24"/>
@@ -9248,6 +9310,11 @@
     <mergeCell ref="B21:B24"/>
     <mergeCell ref="B25:B27"/>
     <mergeCell ref="A3:A9"/>
+    <mergeCell ref="D5:D7"/>
+    <mergeCell ref="B3:B9"/>
+    <mergeCell ref="C11:C14"/>
+    <mergeCell ref="B10:B14"/>
+    <mergeCell ref="B15:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -9258,9 +9325,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H167"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A164" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B167" sqref="B167"/>
+    <sheetView topLeftCell="C1" zoomScale="107" zoomScaleNormal="107" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9281,7 +9348,7 @@
         <v>63</v>
       </c>
       <c r="B1" s="17" t="s">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="C1" s="17" t="s">
         <v>342</v>
@@ -9289,7 +9356,7 @@
     </row>
     <row r="2" spans="1:3" s="23" customFormat="1" ht="306.60000000000002" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="20"/>
-      <c r="B2" s="56" t="s">
+      <c r="B2" s="53" t="s">
         <v>489</v>
       </c>
       <c r="C2" s="22" t="s">
@@ -9298,7 +9365,7 @@
     </row>
     <row r="3" spans="1:3" s="23" customFormat="1" ht="331.2" x14ac:dyDescent="0.3">
       <c r="A3" s="20"/>
-      <c r="B3" s="57"/>
+      <c r="B3" s="54"/>
       <c r="C3" s="22" t="s">
         <v>643</v>
       </c>
@@ -9448,18 +9515,18 @@
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B20" s="14" t="s">
+        <v>696</v>
+      </c>
+      <c r="C20" s="14" t="s">
         <v>697</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>698</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="43.2" x14ac:dyDescent="0.3">
       <c r="B21" s="14" t="s">
+        <v>698</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>699</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>700</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="409.6" x14ac:dyDescent="0.3">
@@ -9488,10 +9555,10 @@
     </row>
     <row r="25" spans="1:4" ht="72" x14ac:dyDescent="0.3">
       <c r="B25" s="14" t="s">
+        <v>671</v>
+      </c>
+      <c r="C25" s="14" t="s">
         <v>672</v>
-      </c>
-      <c r="C25" s="14" t="s">
-        <v>673</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="26.4" x14ac:dyDescent="0.3">
@@ -9581,7 +9648,7 @@
         <v>8</v>
       </c>
       <c r="C37" s="14" t="s">
-        <v>675</v>
+        <v>674</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -9758,7 +9825,7 @@
         <v>46</v>
       </c>
       <c r="C57" s="14" t="s">
-        <v>674</v>
+        <v>673</v>
       </c>
     </row>
     <row r="58" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -9971,10 +10038,10 @@
     </row>
     <row r="87" spans="2:3" ht="57.6" x14ac:dyDescent="0.3">
       <c r="B87" s="14" t="s">
+        <v>665</v>
+      </c>
+      <c r="C87" s="14" t="s">
         <v>666</v>
-      </c>
-      <c r="C87" s="14" t="s">
-        <v>667</v>
       </c>
     </row>
     <row r="88" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
@@ -10124,7 +10191,7 @@
         <v>508</v>
       </c>
       <c r="C108" s="14" t="s">
-        <v>740</v>
+        <v>739</v>
       </c>
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.3">
@@ -10299,10 +10366,10 @@
     </row>
     <row r="134" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B134" s="14" t="s">
+        <v>668</v>
+      </c>
+      <c r="C134" s="14" t="s">
         <v>669</v>
-      </c>
-      <c r="C134" s="14" t="s">
-        <v>670</v>
       </c>
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.3">
@@ -10368,7 +10435,7 @@
         <v>334</v>
       </c>
       <c r="C146" s="14" t="s">
-        <v>668</v>
+        <v>667</v>
       </c>
     </row>
     <row r="147" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
@@ -10376,12 +10443,12 @@
         <v>335</v>
       </c>
       <c r="C147" s="14" t="s">
-        <v>665</v>
+        <v>664</v>
       </c>
     </row>
     <row r="148" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
       <c r="B148" s="14" t="s">
-        <v>741</v>
+        <v>740</v>
       </c>
       <c r="C148" s="14" t="s">
         <v>429</v>
@@ -10411,106 +10478,6 @@
         <v>428</v>
       </c>
     </row>
-    <row r="152" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A152" s="53" t="s">
-        <v>470</v>
-      </c>
-      <c r="B152" s="54"/>
-      <c r="C152" s="55"/>
-    </row>
-    <row r="153" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B153" s="14" t="s">
-        <v>403</v>
-      </c>
-      <c r="C153" s="14" t="s">
-        <v>404</v>
-      </c>
-    </row>
-    <row r="154" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B154" s="14" t="s">
-        <v>405</v>
-      </c>
-      <c r="C154" s="14" t="s">
-        <v>406</v>
-      </c>
-    </row>
-    <row r="155" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B155" s="14" t="s">
-        <v>407</v>
-      </c>
-      <c r="C155" s="14" t="s">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="156" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B156" s="14" t="s">
-        <v>409</v>
-      </c>
-      <c r="C156" s="14" t="s">
-        <v>410</v>
-      </c>
-    </row>
-    <row r="157" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B157" s="14" t="s">
-        <v>411</v>
-      </c>
-      <c r="C157" s="14" t="s">
-        <v>412</v>
-      </c>
-    </row>
-    <row r="158" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B158" s="14" t="s">
-        <v>413</v>
-      </c>
-      <c r="C158" s="14" t="s">
-        <v>414</v>
-      </c>
-    </row>
-    <row r="159" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="B159" s="14" t="s">
-        <v>415</v>
-      </c>
-      <c r="C159" s="14" t="s">
-        <v>416</v>
-      </c>
-    </row>
-    <row r="160" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
-      <c r="B160" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C160" s="14" t="s">
-        <v>662</v>
-      </c>
-    </row>
-    <row r="161" spans="2:3" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="C161" s="14" t="s">
-        <v>658</v>
-      </c>
-    </row>
-    <row r="162" spans="2:3" ht="144" x14ac:dyDescent="0.3">
-      <c r="B162" s="14" t="s">
-        <v>659</v>
-      </c>
-      <c r="C162" s="14" t="s">
-        <v>661</v>
-      </c>
-    </row>
-    <row r="163" spans="2:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="B163" s="14" t="s">
-        <v>417</v>
-      </c>
-      <c r="C163" s="14" t="s">
-        <v>418</v>
-      </c>
-    </row>
-    <row r="164" spans="2:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B164" s="14" t="s">
-        <v>423</v>
-      </c>
-      <c r="C164" s="14" t="s">
-        <v>424</v>
-      </c>
-    </row>
     <row r="165" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B165" s="14" t="s">
         <v>482</v>
@@ -10529,12 +10496,11 @@
     </row>
     <row r="167" spans="2:3" x14ac:dyDescent="0.3">
       <c r="B167" s="14" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="A152:C152"/>
+  <mergeCells count="1">
     <mergeCell ref="B2:B3"/>
   </mergeCells>
   <hyperlinks>
@@ -10550,6 +10516,149 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{78963A04-6EC4-4EB8-BCC6-83A9586D8A06}">
+  <dimension ref="A1:C14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="99" zoomScaleNormal="99" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="57.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>700</v>
+      </c>
+      <c r="C1" s="58" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="59" t="s">
+        <v>470</v>
+      </c>
+      <c r="B2" s="60"/>
+      <c r="C2" s="61"/>
+    </row>
+    <row r="3" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
+      <c r="A3" s="19"/>
+      <c r="B3" s="14" t="s">
+        <v>403</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="19"/>
+      <c r="B4" s="14" t="s">
+        <v>405</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="19"/>
+      <c r="B5" s="14" t="s">
+        <v>407</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="19"/>
+      <c r="B6" s="14" t="s">
+        <v>409</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" s="19"/>
+      <c r="B7" s="14" t="s">
+        <v>411</v>
+      </c>
+      <c r="C7" s="14" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8" s="19"/>
+      <c r="B8" s="14" t="s">
+        <v>413</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>414</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A9" s="19"/>
+      <c r="B9" s="14" t="s">
+        <v>415</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="409.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="19"/>
+      <c r="B10" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>743</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="19"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14" t="s">
+        <v>658</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="244.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="19"/>
+      <c r="B12" s="14" t="s">
+        <v>659</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>661</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="19"/>
+      <c r="B13" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>418</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="72" x14ac:dyDescent="0.3">
+      <c r="A14" s="19"/>
+      <c r="B14" s="14" t="s">
+        <v>423</v>
+      </c>
+      <c r="C14" s="14" t="s">
+        <v>424</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:C2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51032E14-0A5D-4151-8C06-445604791B52}">
   <dimension ref="A1:B64"/>
   <sheetViews>
@@ -10581,7 +10690,7 @@
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" s="58" t="s">
+      <c r="A6" s="55" t="s">
         <v>568</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -10589,197 +10698,197 @@
       </c>
     </row>
     <row r="7" spans="1:2" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="58"/>
+      <c r="A7" s="55"/>
       <c r="B7" s="11" t="s">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="55"/>
+      <c r="B8" s="43" t="s">
+        <v>693</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
+      <c r="A9" s="55"/>
+      <c r="B9" s="11" t="s">
+        <v>683</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="55"/>
+      <c r="B10" s="11"/>
+    </row>
+    <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A11" s="55"/>
+      <c r="B11" s="11" t="s">
+        <v>675</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="55"/>
+      <c r="B12" s="10" t="s">
+        <v>676</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="55"/>
+      <c r="B13" s="10"/>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="55"/>
+      <c r="B14" s="10" t="s">
+        <v>677</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="55"/>
+      <c r="B15" s="10"/>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A16" s="55"/>
+      <c r="B16" s="11"/>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A17" s="55"/>
+      <c r="B17" s="10"/>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A18" s="55"/>
+      <c r="B18" s="10"/>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A19" s="55"/>
+      <c r="B19" s="10"/>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A20" s="55"/>
+      <c r="B20" s="10"/>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A21" s="55"/>
+      <c r="B21" s="10"/>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A22" s="55"/>
+      <c r="B22" s="10"/>
+    </row>
+    <row r="24" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
+      <c r="A24" s="56" t="s">
+        <v>569</v>
+      </c>
+      <c r="B24" s="11" t="s">
         <v>679</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="58"/>
-      <c r="B8" s="43" t="s">
-        <v>694</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="158.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="58"/>
-      <c r="B9" s="11" t="s">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A25" s="56"/>
+      <c r="B25" s="11"/>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A26" s="56"/>
+      <c r="B26" s="10"/>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A27" s="56"/>
+      <c r="B27" s="10" t="s">
+        <v>682</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A28" s="56"/>
+      <c r="B28" s="10"/>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A29" s="56"/>
+      <c r="B29" s="10"/>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A30" s="56"/>
+      <c r="B30" s="10" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A31" s="56"/>
+      <c r="B31" s="10"/>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A32" s="56"/>
+      <c r="B32" s="10"/>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A33" s="56"/>
+      <c r="B33" s="10" t="s">
+        <v>681</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A34" s="56"/>
+      <c r="B34" s="10"/>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A35" s="56"/>
+      <c r="B35" s="10"/>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A36" s="56"/>
+      <c r="B36" s="10" t="s">
         <v>684</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A10" s="58"/>
-      <c r="B10" s="11"/>
-    </row>
-    <row r="11" spans="1:2" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A11" s="58"/>
-      <c r="B11" s="11" t="s">
-        <v>676</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A12" s="58"/>
-      <c r="B12" s="10" t="s">
-        <v>677</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A13" s="58"/>
-      <c r="B13" s="10"/>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A14" s="58"/>
-      <c r="B14" s="10" t="s">
-        <v>678</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A15" s="58"/>
-      <c r="B15" s="10"/>
-    </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A16" s="58"/>
-      <c r="B16" s="11"/>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="58"/>
-      <c r="B17" s="10"/>
-    </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A18" s="58"/>
-      <c r="B18" s="10"/>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A19" s="58"/>
-      <c r="B19" s="10"/>
-    </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A20" s="58"/>
-      <c r="B20" s="10"/>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A21" s="58"/>
-      <c r="B21" s="10"/>
-    </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A22" s="58"/>
-      <c r="B22" s="10"/>
-    </row>
-    <row r="24" spans="1:2" ht="57.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="59" t="s">
-        <v>569</v>
-      </c>
-      <c r="B24" s="11" t="s">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A25" s="59"/>
-      <c r="B25" s="11"/>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A26" s="59"/>
-      <c r="B26" s="10"/>
-    </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A27" s="59"/>
-      <c r="B27" s="10" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A28" s="59"/>
-      <c r="B28" s="10"/>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A29" s="59"/>
-      <c r="B29" s="10"/>
-    </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A30" s="59"/>
-      <c r="B30" s="10" t="s">
-        <v>681</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A31" s="59"/>
-      <c r="B31" s="10"/>
-    </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A32" s="59"/>
-      <c r="B32" s="10"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A33" s="59"/>
-      <c r="B33" s="10" t="s">
-        <v>682</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A34" s="59"/>
-      <c r="B34" s="10"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A35" s="59"/>
-      <c r="B35" s="10"/>
-    </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A36" s="59"/>
-      <c r="B36" s="10" t="s">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A37" s="56"/>
+      <c r="B37" s="10"/>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A38" s="56"/>
+      <c r="B38" s="10"/>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A39" s="56"/>
+      <c r="B39" s="10" t="s">
         <v>685</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A37" s="59"/>
-      <c r="B37" s="10"/>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A38" s="59"/>
-      <c r="B38" s="10"/>
-    </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A39" s="59"/>
-      <c r="B39" s="10" t="s">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A40" s="56"/>
+      <c r="B40" s="10"/>
+    </row>
+    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A41" s="56"/>
+      <c r="B41" s="10"/>
+    </row>
+    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A42" s="56"/>
+      <c r="B42" s="10" t="s">
         <v>686</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A40" s="59"/>
-      <c r="B40" s="10"/>
-    </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A41" s="59"/>
-      <c r="B41" s="10"/>
-    </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A42" s="59"/>
-      <c r="B42" s="10" t="s">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A43" s="56"/>
+      <c r="B43" s="10"/>
+    </row>
+    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A44" s="56"/>
+      <c r="B44" s="10"/>
+    </row>
+    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A45" s="56"/>
+      <c r="B45" s="10" t="s">
         <v>687</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A43" s="59"/>
-      <c r="B43" s="10"/>
-    </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A44" s="59"/>
-      <c r="B44" s="10"/>
-    </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A45" s="59"/>
-      <c r="B45" s="10" t="s">
-        <v>688</v>
-      </c>
-    </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A46" s="59"/>
+      <c r="A46" s="56"/>
       <c r="B46" s="10"/>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A47" s="59"/>
+      <c r="A47" s="56"/>
       <c r="B47" s="10"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A49" s="58" t="s">
+      <c r="A49" s="55" t="s">
         <v>570</v>
       </c>
       <c r="B49" s="10" t="s">
@@ -10787,73 +10896,73 @@
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A50" s="58"/>
+      <c r="A50" s="55"/>
       <c r="B50" s="10"/>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A51" s="58"/>
+      <c r="A51" s="55"/>
       <c r="B51" s="10" t="s">
+        <v>688</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A52" s="55"/>
+      <c r="B52" s="10"/>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A53" s="55"/>
+      <c r="B53" s="10"/>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A54" s="55"/>
+      <c r="B54" s="10" t="s">
+        <v>690</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A55" s="55"/>
+      <c r="B55" s="10"/>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A56" s="55"/>
+      <c r="B56" s="10"/>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" s="55"/>
+      <c r="B57" s="10" t="s">
         <v>689</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A52" s="58"/>
-      <c r="B52" s="10"/>
-    </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A53" s="58"/>
-      <c r="B53" s="10"/>
-    </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A54" s="58"/>
-      <c r="B54" s="10" t="s">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" s="55"/>
+      <c r="B58" s="10"/>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" s="55"/>
+      <c r="B59" s="10"/>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" s="55"/>
+      <c r="B60" s="10" t="s">
         <v>691</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A55" s="58"/>
-      <c r="B55" s="10"/>
-    </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A56" s="58"/>
-      <c r="B56" s="10"/>
-    </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A57" s="58"/>
-      <c r="B57" s="10" t="s">
-        <v>690</v>
-      </c>
-    </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A58" s="58"/>
-      <c r="B58" s="10"/>
-    </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A59" s="58"/>
-      <c r="B59" s="10"/>
-    </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A60" s="58"/>
-      <c r="B60" s="10" t="s">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" s="55"/>
+      <c r="B61" s="10"/>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" s="55"/>
+      <c r="B62" s="10"/>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" s="55"/>
+      <c r="B63" s="10" t="s">
         <v>692</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A61" s="58"/>
-      <c r="B61" s="10"/>
-    </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A62" s="58"/>
-      <c r="B62" s="10"/>
-    </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A63" s="58"/>
-      <c r="B63" s="10" t="s">
-        <v>693</v>
-      </c>
-    </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A64" s="58"/>
+      <c r="A64" s="55"/>
       <c r="B64" s="10"/>
     </row>
   </sheetData>
@@ -10867,7 +10976,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C55"/>
   <sheetViews>
@@ -11030,7 +11139,7 @@
         <v>174</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>671</v>
+        <v>670</v>
       </c>
     </row>
     <row r="15" spans="1:3" ht="100.8" x14ac:dyDescent="0.3">
@@ -11445,7 +11554,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C21"/>
   <sheetViews>
@@ -11615,7 +11724,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>742</v>
+        <v>741</v>
       </c>
       <c r="C15" s="11" t="s">
         <v>538</v>
@@ -11684,7 +11793,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C70"/>
   <sheetViews>
@@ -12355,7 +12464,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AF2A579C-C456-4994-AC03-9F2365E2E7CB}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -12399,43 +12508,4 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId2"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8385B5A8-9213-481B-8B93-B8B0D707D64F}">
-  <dimension ref="A1:C2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="1" max="1" width="4.88671875" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="28.77734375" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="B1" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="12" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>394</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>